<commit_message>
feat: enhance player statistics tracking and reporting; update CSV and Excel export functionality
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="League Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cyclones" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="League Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Player Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="cyclones" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -494,22 +495,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.543</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.543</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.343</t>
         </is>
       </c>
     </row>
@@ -524,7 +525,613 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="8" customWidth="1" min="10" max="10"/>
+    <col width="8" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>OBP</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>SLG</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>RBI</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2.333</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bryce</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1.500</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cory</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Devon</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.250</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kap</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1.334</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kyla</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1.750</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Rafael</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Stephen</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>cyclones</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -843,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -945,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -1172,6 +1779,57 @@
       <c r="M12" t="inlineStr">
         <is>
           <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TEAM TOTALS</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>35</v>
+      </c>
+      <c r="C13" t="n">
+        <v>19</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11</v>
+      </c>
+      <c r="I13" t="n">
+        <v>11</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>1.343</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add reparse-all option to CLI, enhance filename parsing, and update tests for case sensitivity and season formatting
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="League Summary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Player Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="cyclones" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Cyclones" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -484,7 +484,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -611,7 +611,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -658,7 +658,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -705,7 +705,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -752,7 +752,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -799,7 +799,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -846,7 +846,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -940,7 +940,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -987,7 +987,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>cyclones</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C12" t="n">

</xml_diff>

<commit_message>
refactor: softball statistics module to use PlateAppearance instead of AtBatAttempt
- Renamed AtBatAttempt class to PlateAppearance and updated related code.
- Modified CSV parser to handle plate appearances instead of at-bat attempts.
- Updated repository methods to save and retrieve plate appearances.
- Adjusted Excel exporter to include new statistics for plate appearances.
- Enhanced player statistics calculations to incorporate plate appearances, walks, and sacrifice flies.
- Updated tests to reflect changes in data structure and ensure functionality.
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -7,9 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="League Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Player Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Cyclones" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Legend" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="League Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Player Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Cyclones" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,82 +436,280 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Team</t>
+          <t>Abbreviation</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Games Played</t>
+          <t>Full Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Total Players</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Team BA</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Team OBP</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Team SLG</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Team OPS</t>
+          <t>Formula</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cyclones</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0.543</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.543</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0.800</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1.343</t>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Plate Appearances</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>AB + BB + SF</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>At Bats</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Total attempts - BB - SF</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Hits</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Total bases gained &gt; 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Singles</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Hits with 1 base</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Doubles</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Hits with 2 bases</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Triples</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Hits with 3 bases</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Home Runs</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hits with 4 bases</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BB</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Walks/Bases on Balls</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Outcome = 'BB'</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sacrifice Flies</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Fly ball outcomes with RBI</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RBI</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Runs Batted In</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Runs scored on play</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Runs Scored</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Runs scored by batter</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Batting Average</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>H / AB</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>OBP</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>On-Base Percentage</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>(H + BB + HBP + SF) / (AB + BB + HBP + SF)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SLG</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Slugging Percentage</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Total Bases / AB</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>On-Base Plus Slugging</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>OBP + SLG</t>
         </is>
       </c>
     </row>
@@ -525,7 +724,132 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Games Played</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total Players</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Team PA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Team BB</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Team SF</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Team BA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Team OBP</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Team SLG</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Team OPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cyclones</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" t="n">
+        <v>36</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>1.343</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,13 +861,19 @@
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
     <col width="8" customWidth="1" min="9" max="9"/>
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -559,47 +889,77 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>AB</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>BB</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>RBI</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>BA</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>OBP</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>SLG</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>OPS</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>HR</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>RBI</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
         </is>
       </c>
     </row>
@@ -620,34 +980,52 @@
       <c r="D2" t="n">
         <v>3</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>2.333</t>
         </is>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -665,36 +1043,54 @@
         <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -709,39 +1105,57 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>0.500</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0.500</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1.500</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -759,36 +1173,54 @@
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -806,36 +1238,54 @@
         <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>3</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>1.250</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>3</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -853,36 +1303,54 @@
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -900,36 +1368,54 @@
         <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>1.334</t>
         </is>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -947,36 +1433,54 @@
         <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E9" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>3</v>
+      </c>
+      <c r="N9" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>1.750</t>
         </is>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -994,36 +1498,54 @@
         <v>3</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1041,36 +1563,54 @@
         <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1088,36 +1628,54 @@
         <v>3</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>2</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1125,13 +1683,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1148,10 +1706,13 @@
     <col width="8" customWidth="1" min="7" max="7"/>
     <col width="8" customWidth="1" min="8" max="8"/>
     <col width="8" customWidth="1" min="9" max="9"/>
-    <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="10" customWidth="1" min="11" max="11"/>
-    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="8" customWidth="1" min="10" max="10"/>
+    <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
     <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1162,60 +1723,75 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>AB</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>1B</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>2B</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>3B</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>HR</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>BB</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>RBI</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>BA</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>OBP</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>SLG</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>OPS</t>
         </is>
@@ -1234,39 +1810,48 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>2.333</t>
         </is>
@@ -1282,16 +1867,16 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1300,24 +1885,33 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
@@ -1330,47 +1924,56 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>0.500</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0.500</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>1.500</t>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>1.333</t>
         </is>
       </c>
     </row>
@@ -1384,13 +1987,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1402,24 +2005,33 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -1435,42 +2047,51 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>1.250</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
@@ -1486,13 +2107,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -1504,24 +2125,33 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -1537,13 +2167,13 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
         <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1552,27 +2182,36 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>1.334</t>
         </is>
@@ -1588,16 +2227,16 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -1606,24 +2245,33 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>1.750</t>
         </is>
@@ -1639,13 +2287,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1654,27 +2302,36 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -1690,7 +2347,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -1710,22 +2367,31 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
@@ -1741,42 +2407,51 @@
         <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
@@ -1789,45 +2464,54 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>36</v>
+      </c>
+      <c r="C13" t="n">
         <v>35</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>19</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>11</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>7</v>
       </c>
-      <c r="F13" t="n">
-        <v>1</v>
-      </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
         <v>11</v>
       </c>
-      <c r="I13" t="n">
+      <c r="L13" t="n">
         <v>11</v>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>0.543</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>0.543</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>0.800</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>1.343</t>
         </is>

</xml_diff>

<commit_message>
chore: update output files for stats.xlsx and stats.db
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -724,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -733,15 +733,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="10" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -762,35 +759,20 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Team PA</t>
+          <t>Team BA</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Team BB</t>
+          <t>Team OBP</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Team SF</t>
+          <t>Team SLG</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Team BA</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Team OBP</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Team SLG</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Team OPS</t>
         </is>
@@ -808,31 +790,22 @@
       <c r="C2" t="n">
         <v>11</v>
       </c>
-      <c r="D2" t="n">
-        <v>36</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>0.543</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.543</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0.800</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
         <is>
           <t>1.343</t>
         </is>

</xml_diff>

<commit_message>
feat: add options to replace existing games and force confirmation in CLI
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -58,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1662,7 +1663,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2430,61 +2431,61 @@
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>TEAM TOTALS</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B14" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C14" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D14" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E14" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F14" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" t="n">
+      <c r="G14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="L13" t="n">
+      <c r="L14" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="M14" s="2" t="inlineStr">
         <is>
           <t>0.543</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="N14" s="2" t="inlineStr">
         <is>
           <t>0.543</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="O14" s="2" t="inlineStr">
         <is>
           <t>0.800</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="P14" s="2" t="inlineStr">
         <is>
           <t>1.343</t>
         </is>

</xml_diff>

<commit_message>
chore: update binary output files for stats and database
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -725,7 +725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -734,46 +734,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="16" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>League</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Team</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Games Played</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Total Players</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Team BA</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Team OBP</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Team SLG</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Team OPS</t>
         </is>
@@ -782,31 +788,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Fray</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Cyclones</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
       <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
         <v>11</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>0.543</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>0.543</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>0.800</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>1.343</t>
         </is>

</xml_diff>

<commit_message>
feat: add autofilter functionality to league and team summary sheets in Excel export
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -12,7 +12,11 @@
     <sheet name="Player Summary" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Cyclones" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'League Summary'!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Player Summary'!$A$1:$Q$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Cyclones'!$A$1:$P$12</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -824,6 +828,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1664,6 +1669,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q12"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2503,6 +2509,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P12"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: player data and update statistics for Pacific and Mountain teams
- Updated player performance data in CSV files for Pacific Sharks and Bears across multiple fall and spring games.
- Removed outdated CSV files for Mountain Bears and Sharks winter games.
- Enhanced the data generation script to include realistic outcome weights for player statistics.
- Modified CLI to allow custom database file paths for better flexibility in data management.
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -10,12 +10,16 @@
     <sheet name="Legend" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="League Summary" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Player Summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Cyclones" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Cyclones Total" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Cyclones Winter 2026 Total" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Cyclones Winter 2026 Game 1" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'League Summary'!$A$1:$H$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Player Summary'!$A$1:$Q$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Cyclones'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Player Summary'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Cyclones Total'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Cyclones Winter 2026 Total'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Cyclones Winter 2026 Game 1'!$A$1:$P$12</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -813,7 +817,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.543</t>
+          <t>0.528</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -823,7 +827,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1.343</t>
+          <t>1.328</t>
         </is>
       </c>
     </row>
@@ -839,7 +843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -848,7 +852,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
@@ -859,11 +863,10 @@
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
-    <col width="8" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
     <col width="10" customWidth="1" min="14" max="14"/>
     <col width="10" customWidth="1" min="15" max="15"/>
     <col width="10" customWidth="1" min="16" max="16"/>
-    <col width="10" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -874,80 +877,75 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Team</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>H</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>1B</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>1B</t>
+          <t>2B</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>2B</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>SF</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>RBI</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>RBI</t>
+          <t>R</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>OBP</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>OBP</t>
+          <t>SLG</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>SLG</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>OPS</t>
         </is>
@@ -959,10 +957,8 @@
           <t>Alex</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B2" t="n">
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>3</v>
@@ -971,13 +967,13 @@
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -989,13 +985,15 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
       </c>
-      <c r="M2" t="n">
-        <v>1</v>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -1004,15 +1002,10 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.333</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
-        <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
         <is>
           <t>2.333</t>
         </is>
@@ -1024,25 +1017,23 @@
           <t>Anthony</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B3" t="n">
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -1057,10 +1048,12 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1069,15 +1062,10 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>1.333</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
-        <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
@@ -1089,25 +1077,23 @@
           <t>Bryce</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B4" t="n">
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -1116,16 +1102,18 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
-      </c>
-      <c r="M4" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1134,17 +1122,12 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>1.333</t>
+          <t>1.500</t>
         </is>
       </c>
     </row>
@@ -1154,22 +1137,20 @@
           <t>Cory</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B5" t="n">
+        <v>3</v>
       </c>
       <c r="C5" t="n">
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1187,10 +1168,12 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1203,11 +1186,6 @@
         </is>
       </c>
       <c r="P5" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -1219,28 +1197,26 @@
           <t>Devon</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B6" t="n">
+        <v>4</v>
       </c>
       <c r="C6" t="n">
         <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1249,13 +1225,15 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
-      </c>
-      <c r="M6" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1264,15 +1242,10 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>1.250</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
-        <is>
-          <t>1.250</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
@@ -1284,22 +1257,20 @@
           <t>Kap</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B7" t="n">
+        <v>3</v>
       </c>
       <c r="C7" t="n">
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1317,10 +1288,12 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1333,11 +1306,6 @@
         </is>
       </c>
       <c r="P7" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -1349,22 +1317,20 @@
           <t>Kunal</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B8" t="n">
+        <v>3</v>
       </c>
       <c r="C8" t="n">
         <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -1379,13 +1345,15 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
       </c>
-      <c r="M8" t="n">
-        <v>1</v>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1398,11 +1366,6 @@
         </is>
       </c>
       <c r="P8" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
         <is>
           <t>1.334</t>
         </is>
@@ -1414,25 +1377,23 @@
           <t>Kyla</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B9" t="n">
+        <v>4</v>
       </c>
       <c r="C9" t="n">
         <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1447,10 +1408,12 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1459,15 +1422,10 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
         <is>
           <t>1.750</t>
         </is>
@@ -1479,22 +1437,20 @@
           <t>Rafael</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B10" t="n">
+        <v>3</v>
       </c>
       <c r="C10" t="n">
         <v>3</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -1509,13 +1465,15 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1528,11 +1486,6 @@
         </is>
       </c>
       <c r="P10" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -1544,16 +1497,14 @@
           <t>Ramos</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B11" t="n">
+        <v>4</v>
       </c>
       <c r="C11" t="n">
         <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1579,8 +1530,10 @@
       <c r="L11" t="n">
         <v>0</v>
       </c>
-      <c r="M11" t="n">
-        <v>0</v>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1593,11 +1546,6 @@
         </is>
       </c>
       <c r="P11" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
@@ -1609,25 +1557,23 @@
           <t>Stephen</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Cyclones</t>
-        </is>
+      <c r="B12" t="n">
+        <v>3</v>
       </c>
       <c r="C12" t="n">
         <v>3</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1639,13 +1585,15 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>2</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1654,22 +1602,17 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>1.333</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
           <t>2.000</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q12"/>
+  <autoFilter ref="A1:P12"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1677,6 +1620,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="FF0000FF"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -1954,9 +1898,850 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>1.500</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cory</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
           <t>0.333</t>
         </is>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Devon</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>1.250</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kap</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>1.334</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kyla</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>1.750</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Rafael</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Stephen</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>TEAM TOTALS</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="M14" s="2" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="N14" s="2" t="inlineStr">
+        <is>
+          <t>0.528</t>
+        </is>
+      </c>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="P14" s="2" t="inlineStr">
+        <is>
+          <t>1.328</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:P12"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="FF00FF00"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="8" customWidth="1" min="10" max="10"/>
+    <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>BB</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>RBI</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>OBP</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>SLG</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>2.333</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bryce</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
       <c r="O4" t="inlineStr">
         <is>
           <t>1.000</t>
@@ -1965,6 +2750,847 @@
       <c r="P4" t="inlineStr">
         <is>
           <t>1.333</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cory</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Devon</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>1.250</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kap</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>1.334</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kyla</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>1.750</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Rafael</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Stephen</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>TEAM TOTALS</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="M14" s="2" t="inlineStr">
+        <is>
+          <t>0.543</t>
+        </is>
+      </c>
+      <c r="N14" s="2" t="inlineStr">
+        <is>
+          <t>0.528</t>
+        </is>
+      </c>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="P14" s="2" t="inlineStr">
+        <is>
+          <t>1.328</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:P12"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="8" customWidth="1" min="10" max="10"/>
+    <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>BB</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>RBI</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>OBP</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>SLG</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>2.333</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bryce</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>1.500</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(exporter): add team name abbreviation for Excel sheet names
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -10,16 +10,18 @@
     <sheet name="Legend" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="League Summary" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Player Summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Cyclones Total" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Cyclones Winter 2026 Total" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Cyclones Winter 2026 Game 1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Cyclo Total" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Cyclo Winter 2026 Total" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Cyclo Winter 2026 Game 1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Cyclo Winter 2026 Game 2" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'League Summary'!$A$1:$H$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Player Summary'!$A$1:$P$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Cyclones Total'!$A$1:$P$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Cyclones Winter 2026 Total'!$A$1:$P$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Cyclones Winter 2026 Game 1'!$A$1:$P$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Player Summary'!$A$1:$Q$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Cyclo Total'!$A$1:$Q$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Cyclo Winter 2026 Total'!$A$1:$Q$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Cyclo Winter 2026 Game 1'!$A$1:$Q$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Cyclo Winter 2026 Game 2'!$A$1:$Q$13</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -437,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -623,100 +625,117 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RBI</t>
+          <t>HRO</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Runs Batted In</t>
+          <t>Home Run Outs</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Runs scored on play</t>
+          <t>Automatic outs from home run rule</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>RBI</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Runs Scored</t>
+          <t>Runs Batted In</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Runs scored by batter</t>
+          <t>Runs scored on play</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>R</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Batting Average</t>
+          <t>Runs Scored</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>H / AB</t>
+          <t>Runs scored by batter</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>OBP</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>On-Base Percentage</t>
+          <t>Batting Average</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>(H + BB + HBP + SF) / (AB + BB + HBP + SF)</t>
+          <t>H / AB</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SLG</t>
+          <t>OBP</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Slugging Percentage</t>
+          <t>On-Base Percentage</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Total Bases / AB</t>
+          <t>(H + BB + HBP + SF) / (AB + BB + HBP + SF)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>SLG</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Slugging Percentage</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Total Bases / AB</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>OPS</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>On-Base Plus Slugging</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>OBP + SLG</t>
         </is>
@@ -796,38 +815,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fray</t>
+          <t>Unknown League</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cyclones</t>
+          <t>No teams found</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.543</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.528</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1.328</t>
+          <t>0.000</t>
         </is>
       </c>
     </row>
@@ -843,7 +862,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -863,10 +882,11 @@
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
     <col width="10" customWidth="1" min="14" max="14"/>
     <col width="10" customWidth="1" min="15" max="15"/>
     <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -922,30 +942,35 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>HRO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>RBI</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>BA</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>OBP</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>SLG</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>OPS</t>
         </is>
@@ -958,16 +983,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -985,29 +1010,32 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2.333</t>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>1.833</t>
         </is>
       </c>
     </row>
@@ -1018,19 +1046,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1039,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -1048,26 +1076,29 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2.000</t>
+          <t>1.500</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2.250</t>
         </is>
       </c>
     </row>
@@ -1078,16 +1109,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -1105,29 +1136,32 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0.500</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>1.500</t>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>1.750</t>
         </is>
       </c>
     </row>
@@ -1138,19 +1172,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1159,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -1168,26 +1202,29 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>1.250</t>
         </is>
       </c>
     </row>
@@ -1198,19 +1235,19 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -1219,35 +1256,38 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>0.750</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.667</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>0.667</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>2.000</t>
+          <t>1.167</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>1.834</t>
         </is>
       </c>
     </row>
@@ -1258,16 +1298,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -1279,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -1288,26 +1328,29 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>1.000</t>
         </is>
       </c>
     </row>
@@ -1318,13 +1361,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
@@ -1333,7 +1376,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1345,29 +1388,32 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.600</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>2.400</t>
         </is>
       </c>
     </row>
@@ -1378,19 +1424,19 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
         <v>4</v>
       </c>
-      <c r="C9" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2</v>
-      </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -1408,46 +1454,49 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>0.750</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>1.750</t>
+          <t>1.250</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2.125</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Rafael</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1465,52 +1514,55 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2.000</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Rafael</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -1528,91 +1580,223 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>1.333</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Stephen</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>2</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>1.400</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2.200</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P12"/>
+  <autoFilter ref="A1:Q14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1624,7 +1808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1644,10 +1828,11 @@
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
     <col width="10" customWidth="1" min="14" max="14"/>
     <col width="10" customWidth="1" min="15" max="15"/>
     <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1703,30 +1888,35 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>HRO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>RBI</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>BA</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>OBP</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>SLG</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>OPS</t>
         </is>
@@ -1739,16 +1929,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -1766,29 +1956,32 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2.333</t>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>1.833</t>
         </is>
       </c>
     </row>
@@ -1799,19 +1992,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1820,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -1829,26 +2022,29 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2.000</t>
+          <t>1.500</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2.250</t>
         </is>
       </c>
     </row>
@@ -1859,16 +2055,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -1886,29 +2082,32 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0.500</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>1.500</t>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>1.750</t>
         </is>
       </c>
     </row>
@@ -1919,19 +2118,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1940,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -1949,26 +2148,29 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>1.250</t>
         </is>
       </c>
     </row>
@@ -1979,19 +2181,19 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -2000,35 +2202,38 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>0.750</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.667</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>0.667</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>2.000</t>
+          <t>1.167</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>1.834</t>
         </is>
       </c>
     </row>
@@ -2039,16 +2244,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2060,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -2069,26 +2274,29 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>1.000</t>
         </is>
       </c>
     </row>
@@ -2099,13 +2307,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
@@ -2114,7 +2322,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -2126,29 +2334,32 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.600</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>2.400</t>
         </is>
       </c>
     </row>
@@ -2159,19 +2370,19 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
         <v>4</v>
       </c>
-      <c r="C9" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2</v>
-      </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -2189,46 +2400,49 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>0.750</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>1.750</t>
+          <t>1.250</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2.125</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Rafael</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -2246,52 +2460,55 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2.000</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Rafael</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -2309,151 +2526,286 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>1.333</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Stephen</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>2</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>1.400</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2.200</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>TEAM TOTALS</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="F14" s="2" t="n">
+      <c r="B16" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="L14" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="M14" s="2" t="inlineStr">
-        <is>
-          <t>0.543</t>
-        </is>
-      </c>
-      <c r="N14" s="2" t="inlineStr">
-        <is>
-          <t>0.528</t>
-        </is>
-      </c>
-      <c r="O14" s="2" t="inlineStr">
-        <is>
-          <t>0.800</t>
-        </is>
-      </c>
-      <c r="P14" s="2" t="inlineStr">
-        <is>
-          <t>1.328</t>
+      <c r="J16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="N16" s="2" t="inlineStr">
+        <is>
+          <t>0.678</t>
+        </is>
+      </c>
+      <c r="O16" s="2" t="inlineStr">
+        <is>
+          <t>0.701</t>
+        </is>
+      </c>
+      <c r="P16" s="2" t="inlineStr">
+        <is>
+          <t>1.034</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>1.735</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P12"/>
+  <autoFilter ref="A1:Q14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2465,7 +2817,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2485,10 +2837,11 @@
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
     <col width="10" customWidth="1" min="14" max="14"/>
     <col width="10" customWidth="1" min="15" max="15"/>
     <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2544,30 +2897,35 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>HRO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>RBI</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>BA</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>OBP</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>SLG</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>OPS</t>
         </is>
@@ -2580,16 +2938,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -2607,29 +2965,32 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2.333</t>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>1.833</t>
         </is>
       </c>
     </row>
@@ -2640,19 +3001,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -2661,7 +3022,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -2670,26 +3031,29 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>0.833</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2.000</t>
+          <t>1.500</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2.333</t>
         </is>
       </c>
     </row>
@@ -2700,16 +3064,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -2727,29 +3091,32 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0.500</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
+          <t>0.600</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>1.333</t>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -2760,19 +3127,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -2781,7 +3148,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -2790,26 +3157,29 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.600</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>1.350</t>
         </is>
       </c>
     </row>
@@ -2820,19 +3190,19 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -2841,35 +3211,38 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>0.750</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.667</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>0.714</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>2.000</t>
+          <t>1.167</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>1.881</t>
         </is>
       </c>
     </row>
@@ -2880,16 +3253,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2901,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -2910,26 +3283,29 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>0.600</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>1.100</t>
         </is>
       </c>
     </row>
@@ -2940,13 +3316,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
@@ -2955,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -2967,29 +3343,32 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.600</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>2.400</t>
         </is>
       </c>
     </row>
@@ -3000,19 +3379,19 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
         <v>4</v>
       </c>
-      <c r="C9" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2</v>
-      </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -3030,46 +3409,49 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>0.750</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>1.750</t>
+          <t>1.250</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2.125</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Rafael</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -3087,52 +3469,55 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>0.333</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2.000</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Rafael</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -3150,151 +3535,286 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>1.333</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Stephen</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>2</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>0.667</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>1.333</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.800</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>1.400</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2.200</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>TEAM TOTALS</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="F14" s="2" t="n">
+      <c r="B16" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="L14" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="M14" s="2" t="inlineStr">
-        <is>
-          <t>0.543</t>
-        </is>
-      </c>
-      <c r="N14" s="2" t="inlineStr">
-        <is>
-          <t>0.528</t>
-        </is>
-      </c>
-      <c r="O14" s="2" t="inlineStr">
-        <is>
-          <t>0.800</t>
-        </is>
-      </c>
-      <c r="P14" s="2" t="inlineStr">
-        <is>
-          <t>1.328</t>
+      <c r="J16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="N16" s="2" t="inlineStr">
+        <is>
+          <t>0.678</t>
+        </is>
+      </c>
+      <c r="O16" s="2" t="inlineStr">
+        <is>
+          <t>0.701</t>
+        </is>
+      </c>
+      <c r="P16" s="2" t="inlineStr">
+        <is>
+          <t>1.034</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>1.735</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P12"/>
+  <autoFilter ref="A1:Q14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3306,7 +3826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3326,10 +3846,11 @@
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
-    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
     <col width="10" customWidth="1" min="14" max="14"/>
     <col width="10" customWidth="1" min="15" max="15"/>
     <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3385,30 +3906,35 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>HRO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>RBI</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>BA</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>OBP</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>SLG</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>OPS</t>
         </is>
@@ -3448,27 +3974,30 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>2.333</t>
         </is>
@@ -3511,24 +4040,27 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
@@ -3568,27 +4100,30 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>0.500</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>0.500</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>1.500</t>
         </is>
@@ -3631,24 +4166,27 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -3688,27 +4226,30 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>1.250</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
@@ -3751,24 +4292,27 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -3808,27 +4352,30 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>1.334</t>
         </is>
@@ -3871,24 +4418,27 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
-      </c>
-      <c r="M9" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>3</v>
+      </c>
+      <c r="N9" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>1.000</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>1.750</t>
         </is>
@@ -3928,27 +4478,30 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>0.333</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>0.666</t>
         </is>
@@ -3993,22 +4546,25 @@
       <c r="L11" t="n">
         <v>0</v>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>0.000</t>
         </is>
@@ -4048,27 +4604,30 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>0.667</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>1.333</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>2.000</t>
         </is>
@@ -4108,34 +4667,983 @@
         <v>1</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L14" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="M14" s="2" t="inlineStr">
+      <c r="M14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="N14" s="2" t="inlineStr">
         <is>
           <t>0.543</t>
         </is>
       </c>
-      <c r="N14" s="2" t="inlineStr">
+      <c r="O14" s="2" t="inlineStr">
         <is>
           <t>0.543</t>
         </is>
       </c>
-      <c r="O14" s="2" t="inlineStr">
+      <c r="P14" s="2" t="inlineStr">
         <is>
           <t>0.800</t>
         </is>
       </c>
-      <c r="P14" s="2" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>1.343</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P12"/>
+  <autoFilter ref="A1:Q12"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="8" customWidth="1" min="10" max="10"/>
+    <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>BB</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>HRO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>RBI</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>OBP</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>SLG</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>1.334</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>3.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bryce</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cory</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>3.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Devon</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>1.500</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kap</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>3.000</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>4.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kyla</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>2</v>
+      </c>
+      <c r="M9" t="n">
+        <v>2</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>1.500</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2.500</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Rafael</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>3</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Stephen</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>1.500</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>2.500</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>2</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>TEAM TOTALS</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="N15" s="2" t="inlineStr">
+        <is>
+          <t>0.875</t>
+        </is>
+      </c>
+      <c r="O15" s="2" t="inlineStr">
+        <is>
+          <t>0.875</t>
+        </is>
+      </c>
+      <c r="P15" s="2" t="inlineStr">
+        <is>
+          <t>1.375</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>2.250</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Q13"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(excel_exporter): enhance league summary sheet with database-driven data retrieval feat(use_cases): add method to get comprehensive league summary data for all teams refactor: update league summary creation logic to handle empty cases and improve data aggregation
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -815,38 +815,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Unknown League</t>
+          <t>Fray</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>No teams found</t>
+          <t>Cyclones</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.678</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.701</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.034</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.735</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor(excel_exporter): clean up summary data construction and improve column handling in sheets
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -2798,7 +2798,7 @@
           <t>1.034</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="Q16" s="2" t="inlineStr">
         <is>
           <t>1.735</t>
         </is>
@@ -3807,7 +3807,7 @@
           <t>1.034</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="Q16" s="2" t="inlineStr">
         <is>
           <t>1.735</t>
         </is>
@@ -4690,7 +4690,7 @@
           <t>0.800</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="Q14" s="2" t="inlineStr">
         <is>
           <t>1.343</t>
         </is>
@@ -5636,7 +5636,7 @@
           <t>1.375</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="Q15" s="2" t="inlineStr">
         <is>
           <t>2.250</t>
         </is>

</xml_diff>

<commit_message>
feat(data): add new player statistics CSV files and update database and Excel output
</commit_message>
<xml_diff>
--- a/data/output/stats.xlsx
+++ b/data/output/stats.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Legend" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="League Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Player Summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Cyclo Total" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Cyclo Winter 2026 Total" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Cyclo Winter 2026 Game 1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Cyclo Winter 2026 Game 2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Legend" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="League Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Player Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cyclo Total" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cyclo Winter 2026 Total" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cyclo Winter 2026 Game 1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cyclo Winter 2026 Game 2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cyclo Winter 2026 Game 3" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'League Summary'!$A$1:$H$2</definedName>
@@ -22,6 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Cyclo Winter 2026 Total'!$A$1:$Q$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Cyclo Winter 2026 Game 1'!$A$1:$Q$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Cyclo Winter 2026 Game 2'!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Cyclo Winter 2026 Game 3'!$A$1:$Q$12</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -824,29 +826,29 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>13</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.678</t>
+          <t>0.611</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.701</t>
+          <t>0.631</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1.034</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1.735</t>
+          <t>1.589</t>
         </is>
       </c>
     </row>
@@ -983,19 +985,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -1016,26 +1018,26 @@
         <v>2</v>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1.833</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -1046,19 +1048,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1076,29 +1078,29 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>5</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
           <t>1.500</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>2.250</t>
         </is>
       </c>
     </row>
@@ -1109,59 +1111,59 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>7</v>
+      </c>
+      <c r="M4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>4</v>
-      </c>
-      <c r="M4" t="n">
-        <v>3</v>
-      </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.571</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>1.750</t>
+          <t>2.428</t>
         </is>
       </c>
     </row>
@@ -1172,25 +1174,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -1202,29 +1204,29 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>1.286</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>1.857</t>
         </is>
       </c>
     </row>
@@ -1235,16 +1237,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -1272,22 +1274,22 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.556</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.556</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>1.167</t>
+          <t>0.889</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>1.834</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -1298,59 +1300,59 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
         <v>4</v>
       </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>2</v>
-      </c>
       <c r="M7" t="n">
         <v>2</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.858</t>
         </is>
       </c>
     </row>
@@ -1361,59 +1363,59 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3</v>
+      </c>
+      <c r="M8" t="n">
         <v>5</v>
       </c>
-      <c r="D8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>2</v>
-      </c>
-      <c r="M8" t="n">
-        <v>3</v>
-      </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>1.375</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2.400</t>
+          <t>2.250</t>
         </is>
       </c>
     </row>
@@ -1424,10 +1426,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
         <v>7</v>
@@ -1461,22 +1463,22 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.875</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>0.875</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2.125</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -1550,19 +1552,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -1580,10 +1582,10 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1597,12 +1599,12 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.400</t>
         </is>
       </c>
     </row>
@@ -1613,16 +1615,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1646,26 +1648,26 @@
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.572</t>
         </is>
       </c>
     </row>
@@ -1739,16 +1741,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1772,26 +1774,26 @@
         <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
           <t>1.000</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>2.000</t>
         </is>
       </c>
     </row>
@@ -1929,19 +1931,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -1962,26 +1964,26 @@
         <v>2</v>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1.833</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -1992,19 +1994,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -2022,29 +2024,29 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>5</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
           <t>1.500</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>2.250</t>
         </is>
       </c>
     </row>
@@ -2055,59 +2057,59 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>7</v>
+      </c>
+      <c r="M4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>4</v>
-      </c>
-      <c r="M4" t="n">
-        <v>3</v>
-      </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.571</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>1.750</t>
+          <t>2.428</t>
         </is>
       </c>
     </row>
@@ -2118,25 +2120,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -2148,29 +2150,29 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>1.286</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>1.857</t>
         </is>
       </c>
     </row>
@@ -2181,16 +2183,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -2218,22 +2220,22 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.556</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.556</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>1.167</t>
+          <t>0.889</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>1.834</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -2244,59 +2246,59 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
         <v>4</v>
       </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>2</v>
-      </c>
       <c r="M7" t="n">
         <v>2</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.858</t>
         </is>
       </c>
     </row>
@@ -2307,59 +2309,59 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3</v>
+      </c>
+      <c r="M8" t="n">
         <v>5</v>
       </c>
-      <c r="D8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>2</v>
-      </c>
-      <c r="M8" t="n">
-        <v>3</v>
-      </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>1.375</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2.400</t>
+          <t>2.250</t>
         </is>
       </c>
     </row>
@@ -2370,10 +2372,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
         <v>7</v>
@@ -2407,22 +2409,22 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.875</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>0.875</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2.125</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -2496,19 +2498,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -2526,10 +2528,10 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -2543,12 +2545,12 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.400</t>
         </is>
       </c>
     </row>
@@ -2559,16 +2561,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -2592,26 +2594,26 @@
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.572</t>
         </is>
       </c>
     </row>
@@ -2685,16 +2687,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -2718,26 +2720,26 @@
         <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
           <t>1.000</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>2.000</t>
         </is>
       </c>
     </row>
@@ -2748,25 +2750,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>3</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>7</v>
@@ -2775,32 +2777,32 @@
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="N16" s="2" t="inlineStr">
         <is>
-          <t>0.678</t>
+          <t>0.611</t>
         </is>
       </c>
       <c r="O16" s="2" t="inlineStr">
         <is>
-          <t>0.701</t>
+          <t>0.631</t>
         </is>
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>1.034</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="Q16" s="2" t="inlineStr">
         <is>
-          <t>1.735</t>
+          <t>1.589</t>
         </is>
       </c>
     </row>
@@ -2938,19 +2940,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -2971,26 +2973,26 @@
         <v>2</v>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1.833</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -3001,19 +3003,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -3031,29 +3033,29 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>5</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.600</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>1.500</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2.333</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -3064,59 +3066,59 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>7</v>
+      </c>
+      <c r="M4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>4</v>
-      </c>
-      <c r="M4" t="n">
-        <v>3</v>
-      </c>
       <c r="N4" t="inlineStr">
         <is>
+          <t>0.857</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
           <t>0.750</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>0.600</t>
-        </is>
-      </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.571</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>2.321</t>
         </is>
       </c>
     </row>
@@ -3127,25 +3129,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -3157,29 +3159,29 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0.600</t>
+          <t>0.625</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>1.286</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>1.350</t>
+          <t>1.911</t>
         </is>
       </c>
     </row>
@@ -3190,16 +3192,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -3227,22 +3229,22 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.556</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>0.714</t>
+          <t>0.600</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>1.167</t>
+          <t>0.889</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>1.881</t>
+          <t>1.489</t>
         </is>
       </c>
     </row>
@@ -3253,59 +3255,59 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
         <v>4</v>
       </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>2</v>
-      </c>
       <c r="M7" t="n">
         <v>2</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
+          <t>0.429</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
           <t>0.500</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>0.600</t>
-        </is>
-      </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.500</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>1.100</t>
+          <t>0.929</t>
         </is>
       </c>
     </row>
@@ -3316,59 +3318,59 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3</v>
+      </c>
+      <c r="M8" t="n">
         <v>5</v>
       </c>
-      <c r="D8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>2</v>
-      </c>
-      <c r="M8" t="n">
-        <v>3</v>
-      </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>1.375</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2.400</t>
+          <t>2.250</t>
         </is>
       </c>
     </row>
@@ -3379,10 +3381,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
         <v>7</v>
@@ -3416,22 +3418,22 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.875</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>0.875</t>
+          <t>0.636</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2.125</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -3505,19 +3507,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -3535,10 +3537,10 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -3552,12 +3554,12 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.400</t>
         </is>
       </c>
     </row>
@@ -3568,16 +3570,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -3601,26 +3603,26 @@
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.286</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.572</t>
         </is>
       </c>
     </row>
@@ -3694,16 +3696,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -3727,26 +3729,26 @@
         <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.667</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.500</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2.000</t>
+          <t>1.167</t>
         </is>
       </c>
     </row>
@@ -3757,25 +3759,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>3</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>7</v>
@@ -3784,32 +3786,32 @@
         <v>1</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="N16" s="2" t="inlineStr">
         <is>
-          <t>0.678</t>
+          <t>0.611</t>
         </is>
       </c>
       <c r="O16" s="2" t="inlineStr">
         <is>
-          <t>0.701</t>
+          <t>0.631</t>
         </is>
       </c>
       <c r="P16" s="2" t="inlineStr">
         <is>
-          <t>1.034</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="Q16" s="2" t="inlineStr">
         <is>
-          <t>1.735</t>
+          <t>1.589</t>
         </is>
       </c>
     </row>
@@ -5646,4 +5648,887 @@
   <autoFilter ref="A1:Q13"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="8" customWidth="1" min="10" max="10"/>
+    <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>3B</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>BB</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>HRO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>RBI</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>OBP</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>SLG</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>OPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>1.250</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.250</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0.250</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0.750</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bryce</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>2.333</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>3.333</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cory</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>2.667</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Devon</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kap</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>2.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kyla</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Rafael</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>1.500</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>2</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0.667</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>1.334</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0.333</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0.666</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>TEAM TOTALS</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="N14" s="2" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <t>0.500</t>
+        </is>
+      </c>
+      <c r="P14" s="2" t="inlineStr">
+        <is>
+          <t>0.833</t>
+        </is>
+      </c>
+      <c r="Q14" s="2" t="inlineStr">
+        <is>
+          <t>1.333</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Q12"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>